<commit_message>
working on gd-ad-1 prob
</commit_message>
<xml_diff>
--- a/stepout_qc_code/write_string/renumeration.xlsx
+++ b/stepout_qc_code/write_string/renumeration.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -959,6 +959,78 @@
         <v>45341</v>
       </c>
       <c r="F20" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>india</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>sri lanka</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>777</v>
+      </c>
+      <c r="D21" t="n">
+        <v>90</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>45344</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>barca</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>6655</v>
+      </c>
+      <c r="D22" t="n">
+        <v>90</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>45344</v>
+      </c>
+      <c r="F22" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ooo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>pppp</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1245</v>
+      </c>
+      <c r="D23" t="n">
+        <v>90</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>45344</v>
+      </c>
+      <c r="F23" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started qc to src
</commit_message>
<xml_diff>
--- a/stepout_qc_code/write_string/renumeration.xlsx
+++ b/stepout_qc_code/write_string/renumeration.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Boni" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Arpit" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sudhanva" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rahul" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1554,4 +1555,79 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>team_a_name</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>team_b_name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>match_id</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>game_time</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>current_date</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>renumeration</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yuu</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>iuu</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>123</v>
+      </c>
+      <c r="D2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>45352</v>
+      </c>
+      <c r="F2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>